<commit_message>
updated ressource results && added runtime results for 6x
</commit_message>
<xml_diff>
--- a/results/2013.09.04_ressource_comparison/ressources.xlsx
+++ b/results/2013.09.04_ressource_comparison/ressources.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="2100" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,23 +14,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>Folder: results</t>
   </si>
   <si>
-    <t>Date: September 02, 2013</t>
-  </si>
-  <si>
     <t>Repository: git@git.rhrk.uni-kl.de:EIT-Wehn/finance.zynqpricer.hls.git</t>
   </si>
   <si>
     <t>Author: Christian Brugger (brugger@eit.uni-kl.de)</t>
   </si>
   <si>
-    <t>Revision: 782133776b0e701ea69b07d6e8d0cb7158f1f543</t>
-  </si>
-  <si>
     <t>Heston SL, Float, Zynq (heston_sl_3x)</t>
   </si>
   <si>
@@ -71,13 +65,31 @@
   </si>
   <si>
     <t>Heston Accelerator</t>
+  </si>
+  <si>
+    <t>Heston SL, Float, Zynq (heston_sl_6x)</t>
+  </si>
+  <si>
+    <t>Date: September 07, 2013</t>
+  </si>
+  <si>
+    <t>ICDF</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Usage [%]</t>
+  </si>
+  <si>
+    <t>Revision: ee9c3b897f8ab2130fb8fffef0426ce060c5c65c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +126,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -132,10 +151,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -147,9 +167,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -451,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -462,64 +485,64 @@
     <col min="1" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="3" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="3" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="3" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:6" s="3" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="3" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="3" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="3" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B10" s="2">
         <v>100</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C12" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="F12" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C13" s="6">
         <v>53200</v>
@@ -536,7 +559,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C14" s="2">
         <v>4458</v>
@@ -553,7 +576,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C15" s="2">
         <v>3611</v>
@@ -570,7 +593,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C16" s="2">
         <v>229</v>
@@ -587,7 +610,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C17" s="2">
         <v>286</v>
@@ -604,7 +627,7 @@
     </row>
     <row r="19" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C19" s="6">
         <f>SUM(C14:C17)</f>
@@ -625,7 +648,7 @@
     </row>
     <row r="20" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C20" s="6">
         <f>1150+300</f>
@@ -641,7 +664,223 @@
         <v>0</v>
       </c>
     </row>
+    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="2">
+        <v>100</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6">
+        <v>53200</v>
+      </c>
+      <c r="D29" s="6">
+        <v>106400</v>
+      </c>
+      <c r="E29" s="6">
+        <v>140</v>
+      </c>
+      <c r="F29" s="6">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="2">
+        <v>4597</v>
+      </c>
+      <c r="D31" s="2">
+        <v>4443</v>
+      </c>
+      <c r="E31" s="2">
+        <v>1</v>
+      </c>
+      <c r="F31" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="2">
+        <v>447</v>
+      </c>
+      <c r="D32" s="2">
+        <v>592</v>
+      </c>
+      <c r="E32" s="2">
+        <v>2</v>
+      </c>
+      <c r="F32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="2">
+        <v>229</v>
+      </c>
+      <c r="D33" s="2">
+        <v>287</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="2">
+        <v>286</v>
+      </c>
+      <c r="D34" s="2">
+        <v>323</v>
+      </c>
+      <c r="E34" s="2">
+        <v>2</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6">
+        <f>SUM(C31:C34)</f>
+        <v>5559</v>
+      </c>
+      <c r="D36" s="6">
+        <f>SUM(D31:D34)</f>
+        <v>5645</v>
+      </c>
+      <c r="E36" s="6">
+        <f t="shared" ref="E36:F36" si="1">SUM(E31:E34)</f>
+        <v>5</v>
+      </c>
+      <c r="F36" s="6">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="6"/>
+      <c r="C37" s="7">
+        <f>1136+92+(831+18)/6</f>
+        <v>1369.5</v>
+      </c>
+      <c r="D37" s="7">
+        <f>647+54+(743+30)/6</f>
+        <v>829.83333333333337</v>
+      </c>
+      <c r="E37" s="6">
+        <v>6</v>
+      </c>
+      <c r="F37" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6">
+        <f>(C36+C37) * 6</f>
+        <v>41571</v>
+      </c>
+      <c r="D39" s="6">
+        <f t="shared" ref="D39:F39" si="2">(D36+D37) * 6</f>
+        <v>38849</v>
+      </c>
+      <c r="E39" s="6">
+        <f t="shared" si="2"/>
+        <v>66</v>
+      </c>
+      <c r="F39" s="6">
+        <f t="shared" si="2"/>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" s="6"/>
+      <c r="C40" s="8">
+        <f>C39/C29</f>
+        <v>0.78140977443609028</v>
+      </c>
+      <c r="D40" s="8">
+        <f t="shared" ref="D40:F40" si="3">D39/D29</f>
+        <v>0.36512218045112782</v>
+      </c>
+      <c r="E40" s="8">
+        <f t="shared" si="3"/>
+        <v>0.47142857142857142</v>
+      </c>
+      <c r="F40" s="8">
+        <f t="shared" si="3"/>
+        <v>0.98181818181818181</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>